<commit_message>
Updated Hour by hour, progress log and ready to go check list due to installation of Nagios
</commit_message>
<xml_diff>
--- a/Ready-to-Go Checklists/Ready-to-Go Checklist for SCP Build 1.0.0.xlsx
+++ b/Ready-to-Go Checklists/Ready-to-Go Checklist for SCP Build 1.0.0.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>Type</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Hour-By-Hour Plan for deploying on 17 February 2019 ready</t>
+  </si>
+  <si>
+    <t>Nagios Monitoring Tool set up and monitoring SCP</t>
   </si>
 </sst>
 </file>
@@ -379,6 +382,20 @@
         <v>6</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="11">
+        <v>43527.0</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="17">
       <c r="C17" s="13"/>
       <c r="D17" s="14"/>

</xml_diff>